<commit_message>
[ParseWikiToBean]添加解析 wiki 为 Java Bean 的工具
同时更新 redmine 的 excel 模板
</commit_message>
<xml_diff>
--- a/ToolsX/spider/redmine/issues.xlsx
+++ b/ToolsX/spider/redmine/issues.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>指派给</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,32 +34,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Glide 图片加载框架分析学习</t>
-    <rPh sb="0" eb="1">
-      <t>ti'huan</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>xin'ban'ben</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>tu'biao</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>X5 Webview 合并检查</t>
-    <rPh sb="0" eb="1">
-      <t>xiu'gai</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>bu'fen</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>di'zhi</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>状态</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -80,15 +54,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>项目</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>linglingbang628</t>
+    <t>630llb</t>
+  </si>
+  <si>
+    <t>社区广场-顶部广告</t>
   </si>
 </sst>
 </file>
@@ -98,7 +71,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +114,38 @@
       <color theme="1"/>
       <name val="微软雅黑"/>
       <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="DengXian"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -195,13 +200,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -226,9 +239,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -238,13 +248,29 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1"/>
+    <cellStyle name="常规 2 2" xfId="2"/>
+    <cellStyle name="常规 3" xfId="3"/>
+    <cellStyle name="常规 4" xfId="4"/>
+    <cellStyle name="常规 5" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -533,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -544,33 +570,33 @@
     <col min="1" max="1" width="13.875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.25" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="72.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.375" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.75" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1"/>
     <col min="8" max="9" width="12.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" style="11"/>
+    <col min="10" max="10" width="9" style="10"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>0</v>
@@ -581,69 +607,119 @@
       <c r="I1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="9">
+      <c r="A2" s="8">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="8">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>4</v>
+      <c r="D2" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2" s="3">
         <v>42</v>
       </c>
       <c r="H2" s="5">
-        <v>43164</v>
+        <v>43273</v>
       </c>
       <c r="I2" s="5">
-        <v>43165</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>11</v>
-      </c>
+        <v>43273</v>
+      </c>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A3" s="9">
-        <v>0</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="9">
-        <v>2</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="6">
-        <v>3</v>
-      </c>
-      <c r="G3" s="3">
-        <v>42</v>
-      </c>
-      <c r="H3" s="5">
-        <v>43166</v>
-      </c>
-      <c r="I3" s="5">
-        <v>43166</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:10" ht="16.5">
+      <c r="D4" s="13"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" ht="16.5">
+      <c r="D5" s="13"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" ht="16.5">
+      <c r="D6" s="13"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" ht="16.5">
+      <c r="D7" s="13"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" ht="16.5">
+      <c r="D8" s="13"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" ht="16.5">
+      <c r="D9" s="12"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" ht="16.5">
+      <c r="D10" s="12"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" ht="16.5">
+      <c r="D11" s="14"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" ht="16.5">
+      <c r="D12" s="14"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" ht="16.5">
+      <c r="D13" s="14"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" ht="16.5">
+      <c r="D14" s="14"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" ht="16.5">
+      <c r="D15" s="14"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" ht="16.5">
+      <c r="D16" s="11"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="4:9" ht="16.5">
+      <c r="D17" s="11"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>